<commit_message>
implementation and improved writing
</commit_message>
<xml_diff>
--- a/src/test/resources/StimaInnovaFase2Sprint2.xlsx
+++ b/src/test/resources/StimaInnovaFase2Sprint2.xlsx
@@ -1272,8 +1272,8 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="32.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1410,13 +1410,15 @@
         <v>64</v>
       </c>
       <c r="D6" s="31"/>
-      <c r="E6" s="25"/>
+      <c r="E6" s="25" t="n">
+        <v>2</v>
+      </c>
       <c r="F6" s="25" t="n">
         <v>5</v>
       </c>
       <c r="G6" s="25" t="n">
         <f aca="false">SUM(E6,F6)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AB6" s="25" t="n">
         <v>3</v>
@@ -1431,13 +1433,15 @@
       <c r="D7" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="25" t="n">
+        <v>1</v>
+      </c>
       <c r="F7" s="25" t="n">
         <v>5</v>
       </c>
       <c r="G7" s="25" t="n">
         <f aca="false">SUM(E7,F7)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB7" s="25" t="n">
         <v>3</v>
@@ -1454,6 +1458,9 @@
         <v>68</v>
       </c>
       <c r="D8" s="31"/>
+      <c r="E8" s="25" t="n">
+        <v>0</v>
+      </c>
       <c r="F8" s="25" t="n">
         <v>5</v>
       </c>
@@ -1495,20 +1502,22 @@
         <v>71</v>
       </c>
       <c r="D10" s="31"/>
-      <c r="E10" s="25"/>
+      <c r="E10" s="25" t="n">
+        <v>9</v>
+      </c>
       <c r="F10" s="25" t="n">
         <v>8</v>
       </c>
       <c r="G10" s="25" t="n">
         <f aca="false">SUM(E10,F10)</f>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="AB10" s="25" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="60.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="32" t="s">
         <v>72</v>
       </c>
       <c r="B11" s="34" t="s">
@@ -1532,7 +1541,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="34" t="s">
         <v>75</v>
       </c>
@@ -1552,7 +1561,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="34" t="s">
         <v>77</v>
       </c>
@@ -1626,12 +1635,15 @@
         <v>85</v>
       </c>
       <c r="D16" s="31"/>
+      <c r="E16" s="25" t="n">
+        <v>5</v>
+      </c>
       <c r="F16" s="25" t="n">
         <v>2</v>
       </c>
       <c r="G16" s="25" t="n">
         <f aca="false">SUM(E16,F16)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="110.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1682,7 +1694,7 @@
       </c>
       <c r="E19" s="38" t="n">
         <f aca="false">SUM(E3:E18)</f>
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F19" s="38" t="n">
         <f aca="false">SUM(F3:F18)</f>
@@ -1690,7 +1702,7 @@
       </c>
       <c r="G19" s="38" t="n">
         <f aca="false">SUM(G3:G17)</f>
-        <v>72</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="32.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>